<commit_message>
change "mouse" to "replicate"
</commit_message>
<xml_diff>
--- a/inst/extdata/PL_D-21_BCG_CFUs.xlsx
+++ b/inst/extdata/PL_D-21_BCG_CFUs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henaolab/Documents/R/test_mycyto/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henaolab/Documents/R/bactcountr/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B057C7-5301-EE42-824D-4205E72E9C24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD7808E-9006-C04A-90DA-766C88283165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>group</t>
   </si>
   <si>
-    <t>mouse</t>
-  </si>
-  <si>
     <t>organ</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>resuspend_volume_mL</t>
+  </si>
+  <si>
+    <t>replicate</t>
   </si>
 </sst>
 </file>
@@ -112,10 +112,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -364,7 +366,7 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="E13" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -374,22 +376,22 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="J1" s="2"/>
     </row>
@@ -398,10 +400,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>26</v>
@@ -422,13 +424,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="1">
         <v>52</v>
@@ -445,10 +447,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -468,10 +470,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -491,16 +493,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1">
         <v>30</v>
@@ -514,10 +516,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -537,10 +539,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -560,10 +562,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -583,10 +585,10 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -606,10 +608,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -629,10 +631,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -652,10 +654,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -675,10 +677,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -698,10 +700,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -721,10 +723,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -744,10 +746,10 @@
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1">
         <v>17</v>
@@ -767,10 +769,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -790,10 +792,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1">
         <v>4</v>
@@ -813,10 +815,10 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -836,10 +838,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -859,10 +861,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -882,10 +884,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -905,10 +907,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -928,10 +930,10 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="1">
         <v>0</v>
@@ -951,10 +953,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" s="1">
         <v>0</v>
@@ -974,10 +976,10 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
@@ -997,10 +999,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1">
         <v>0</v>
@@ -1020,10 +1022,10 @@
         <v>3</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -1043,10 +1045,10 @@
         <v>3</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1">
         <v>0</v>
@@ -1066,10 +1068,10 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" s="1">
         <v>0</v>
@@ -1089,10 +1091,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1">
         <v>0</v>
@@ -1112,10 +1114,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D33" s="1">
         <v>0</v>
@@ -1135,10 +1137,10 @@
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D34" s="1">
         <v>0</v>
@@ -1158,10 +1160,10 @@
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="1">
         <v>0</v>
@@ -1181,10 +1183,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" s="1">
         <v>0</v>
@@ -1204,10 +1206,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -1227,10 +1229,10 @@
         <v>7</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38" s="1">
         <v>0</v>
@@ -1250,10 +1252,10 @@
         <v>7</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" s="1">
         <v>0</v>
@@ -1273,10 +1275,10 @@
         <v>8</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" s="1">
         <v>0</v>
@@ -1296,10 +1298,10 @@
         <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" s="1">
         <v>0</v>
@@ -1319,10 +1321,10 @@
         <v>8</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D42" s="2">
         <v>1</v>
@@ -1342,10 +1344,10 @@
         <v>9</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D43" s="1">
         <v>0</v>
@@ -1365,10 +1367,10 @@
         <v>9</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D44" s="1">
         <v>0</v>
@@ -1388,10 +1390,10 @@
         <v>9</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" s="1">
         <v>0</v>
@@ -1411,10 +1413,10 @@
         <v>10</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" s="1">
         <v>0</v>
@@ -1434,10 +1436,10 @@
         <v>10</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D47" s="1">
         <v>0</v>
@@ -1490,10 +1492,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">

</xml_diff>